<commit_message>
results 변경 및 new_results 삭제
</commit_message>
<xml_diff>
--- a/python_engine/data/input/시나리오_공정제약조건.xlsx
+++ b/python_engine/data/input/시나리오_공정제약조건.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\OneDrive\바탕 화면\생산계획\스케줄링-0923 (local-updates branch)\python_engine\data\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kim\OneDrive\바탕 화면\생산계획\스케줄링-1112\python_engine\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60CA1134-D8B4-417C-A4B8-3A97201556F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFC4AD5C-A7D4-45B6-8A9D-D5AA8E982666}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15030" yWindow="-13845" windowWidth="11970" windowHeight="11295" firstSheet="1" activeTab="2" xr2:uid="{7E8ADE5F-D31F-4BDE-9BF4-6FC4B9644929}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15720" firstSheet="1" activeTab="2" xr2:uid="{7E8ADE5F-D31F-4BDE-9BF4-6FC4B9644929}"/>
   </bookViews>
   <sheets>
     <sheet name="machine_limit" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>proccode</t>
   </si>
@@ -51,6 +51,10 @@
   </si>
   <si>
     <t>rest_end</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>C2010</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -119,12 +123,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,13 +515,16 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{336928BA-28AA-4137-A7A8-07C56A4674DF}">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="3" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -525,6 +535,17 @@
       </c>
       <c r="C1" s="1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2">
+        <v>45792</v>
+      </c>
+      <c r="C2" s="2">
+        <v>45807</v>
       </c>
     </row>
   </sheetData>

</xml_diff>